<commit_message>
Some changes done to the code
</commit_message>
<xml_diff>
--- a/CURA-PRACTICE/TestData/CuraHealthData.xlsx
+++ b/CURA-PRACTICE/TestData/CuraHealthData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rakesh.sd\eclipse-workspace\CURA-PRACTICE\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rakesh\eclipse-workspace\CURA-PRACTICE\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1409FC31-38F4-417A-9163-23E8273EBA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C89B11-475C-4E75-B29F-2B447121DF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
   <si>
     <t>UserName</t>
   </si>
@@ -376,12 +376,12 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -395,7 +395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
@@ -406,10 +406,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
         <v>7</v>
       </c>
@@ -420,10 +420,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Final changes based on Selenium done
</commit_message>
<xml_diff>
--- a/CURA-PRACTICE/TestData/CuraHealthData.xlsx
+++ b/CURA-PRACTICE/TestData/CuraHealthData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rakesh\eclipse-workspace\CURA-PRACTICE\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C89B11-475C-4E75-B29F-2B447121DF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B605F932-F5A1-4B35-912E-71DFB5154161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,7 +406,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -420,7 +420,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>